<commit_message>
all the default values have ben added
</commit_message>
<xml_diff>
--- a/django_project/wfrp/example_media/default_armour.xlsx
+++ b/django_project/wfrp/example_media/default_armour.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t xml:space="preserve">character</t>
   </si>
@@ -40,16 +40,43 @@
     <t xml:space="preserve">qualities</t>
   </si>
   <si>
-    <t xml:space="preserve">GUNNAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test shield</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cool</t>
+    <t xml:space="preserve">SALUNDRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full Leather Armour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Breastplate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Body</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOLRELLA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leather Jack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMRIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scale Hauberk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Body, legs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELSE</t>
   </si>
 </sst>
 </file>
@@ -59,7 +86,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -80,6 +107,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -124,12 +156,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -150,13 +186,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.04"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -179,22 +219,122 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="E2" s="0" t="n">
+      <c r="D2" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="C3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>